<commit_message>
allcohorts_1plate_class csv file updated
</commit_message>
<xml_diff>
--- a/Working Files/allcohorts_1plate_familysummarycounts.xlsx
+++ b/Working Files/allcohorts_1plate_familysummarycounts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tan14n\Documents\Github\ViralTransmission\Working Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D40B3816-6B93-42B0-AD6E-BD02A303F291}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D36DA08-5D7C-4E64-8444-203DC1C3C2C0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{19FC6DE0-999F-432F-82D4-554EB798C6B2}"/>
+    <workbookView xWindow="-28920" yWindow="-90" windowWidth="29040" windowHeight="17640" xr2:uid="{19FC6DE0-999F-432F-82D4-554EB798C6B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -675,8 +675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2226411-EF9F-475F-92A7-62B8CD094FF5}">
   <dimension ref="A1:H90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="C95" sqref="C95"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>